<commit_message>
added performance boot changes
</commit_message>
<xml_diff>
--- a/utilities/default_annotations.xlsx
+++ b/utilities/default_annotations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/haavartl_ntnu_no/Documents/Bioinformatikk/coco/utilities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\havar\OneDrive - NTNU\Bioinformatikk\coco\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{0CAC6F51-F52C-4DDB-AFD3-85DE57026C04}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="14_{0CAC6F51-F52C-4DDB-AFD3-85DE57026C04}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{92610CEC-983F-4A60-BA58-F9114CBC8ADB}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="3435" windowWidth="31995" windowHeight="15195" activeTab="1" xr2:uid="{19ECA98E-40E3-4130-97FB-5DA5E4DBFBDF}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="25440" windowHeight="15075" activeTab="1" xr2:uid="{19ECA98E-40E3-4130-97FB-5DA5E4DBFBDF}"/>
   </bookViews>
   <sheets>
     <sheet name="test_settings" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>contrast</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>0,0,255</t>
+  </si>
+  <si>
+    <t>global_max</t>
+  </si>
+  <si>
+    <t>min_size</t>
   </si>
 </sst>
 </file>
@@ -431,21 +437,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B611F2-F3A8-49C0-9E98-254A0A9E298A}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,8 +476,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -491,7 +503,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E3">
         <v>5</v>
       </c>
@@ -502,7 +514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E4">
         <v>20</v>
       </c>
@@ -520,178 +532,186 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A44B0D-BE97-43B7-8D49-3576171B57DB}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
       <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="b">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>255</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>3</v>
       </c>
-      <c r="J2" t="b">
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="L2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="b">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>255</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
       <c r="H3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
-      <c r="J3" t="b">
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="L3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>255</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>3</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>5</v>
       </c>
-      <c r="J4" t="b">
+      <c r="L4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="b">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>7</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>255</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>10</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
       </c>
       <c r="I5">
         <v>3</v>
       </c>
-      <c r="J5" t="b">
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="L5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -707,6 +727,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AAC28648A522184EA36A2635563BFE17" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="740788dfa5b919fc9e8d7dbe9f7dd0b6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a610463c-cf77-4be4-9cab-a37d6e5b2b79" xmlns:ns4="70404a6c-3db2-4fe3-97dd-ea7ac57d8e39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed8226736557a80de783c2345303b4e7" ns3:_="" ns4:_="">
     <xsd:import namespace="a610463c-cf77-4be4-9cab-a37d6e5b2b79"/>
@@ -915,15 +944,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0096214C-5DF6-4298-A683-BA2B02940D65}">
   <ds:schemaRefs>
@@ -942,6 +962,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B87E13E-058F-4374-9A26-8CE017B0EDD9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{312C7EE8-74BA-45EE-BA24-E6A3FC861223}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -958,12 +986,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B87E13E-058F-4374-9A26-8CE017B0EDD9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed image ratio issue coco_plot_images
</commit_message>
<xml_diff>
--- a/utilities/default_annotations.xlsx
+++ b/utilities/default_annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\havar\OneDrive - NTNU\Bioinformatikk\coco\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="14_{0CAC6F51-F52C-4DDB-AFD3-85DE57026C04}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{92610CEC-983F-4A60-BA58-F9114CBC8ADB}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="14_{0CAC6F51-F52C-4DDB-AFD3-85DE57026C04}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{21E9B40E-E155-4335-923D-AFDFB91B23DD}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="25440" windowHeight="15075" activeTab="1" xr2:uid="{19ECA98E-40E3-4130-97FB-5DA5E4DBFBDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{19ECA98E-40E3-4130-97FB-5DA5E4DBFBDF}"/>
   </bookViews>
   <sheets>
     <sheet name="test_settings" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>contrast</t>
   </si>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B611F2-F3A8-49C0-9E98-254A0A9E298A}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +482,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -500,6 +500,9 @@
         <v>8</v>
       </c>
       <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -534,7 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A44B0D-BE97-43B7-8D49-3576171B57DB}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -727,15 +730,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AAC28648A522184EA36A2635563BFE17" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="740788dfa5b919fc9e8d7dbe9f7dd0b6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a610463c-cf77-4be4-9cab-a37d6e5b2b79" xmlns:ns4="70404a6c-3db2-4fe3-97dd-ea7ac57d8e39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed8226736557a80de783c2345303b4e7" ns3:_="" ns4:_="">
     <xsd:import namespace="a610463c-cf77-4be4-9cab-a37d6e5b2b79"/>
@@ -944,6 +938,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0096214C-5DF6-4298-A683-BA2B02940D65}">
   <ds:schemaRefs>
@@ -962,14 +965,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B87E13E-058F-4374-9A26-8CE017B0EDD9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{312C7EE8-74BA-45EE-BA24-E6A3FC861223}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -986,4 +981,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B87E13E-058F-4374-9A26-8CE017B0EDD9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>